<commit_message>
minor update to ODK form
</commit_message>
<xml_diff>
--- a/odk/TAPE - WIP.xlsx
+++ b/odk/TAPE - WIP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/SSD Dropbox/Stats4SD Projects/ICRAF -TAPE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Projects/Rstudio/tape_calculator/odk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86566FCD-3604-E144-AB6A-596B08561AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8B55BD-9CD3-AA45-9420-6544BB8DEE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15760" yWindow="-28300" windowWidth="39920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6223" uniqueCount="3198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6224" uniqueCount="3199">
   <si>
     <t>Comment</t>
   </si>
@@ -9700,6 +9700,9 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maybe don't need this any more? </t>
   </si>
 </sst>
 </file>
@@ -10828,11 +10831,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1067"/>
   <sheetViews>
-    <sheetView zoomScale="178" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -11115,8 +11118,10 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:15" ht="16">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:15" ht="64">
+      <c r="A15" s="1" t="s">
+        <v>3198</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -28115,7 +28120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1720"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+    <sheetView zoomScale="162" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A604" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B608" sqref="B608"/>
     </sheetView>

</xml_diff>

<commit_message>
move to 1.2 of excel-to-csv action
</commit_message>
<xml_diff>
--- a/odk/TAPE - WIP.xlsx
+++ b/odk/TAPE - WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Projects/Rstudio/tape_calculator/odk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC310C9-D87C-E54C-87E6-E91B60309B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F00789-B0C1-054C-8807-AF9493A29966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15760" yWindow="-28300" windowWidth="39920" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6223" uniqueCount="3198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6224" uniqueCount="3199">
   <si>
     <t>Comment</t>
   </si>
@@ -9700,6 +9700,9 @@
   </si>
   <si>
     <t xml:space="preserve">maybe don't need this any more? </t>
+  </si>
+  <si>
+    <t>depending on how we approach this section, this could be deleted…</t>
   </si>
 </sst>
 </file>
@@ -10829,10 +10832,10 @@
   <dimension ref="A1:O1067"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -12559,7 +12562,9 @@
       <c r="O80" s="7"/>
     </row>
     <row r="81" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A81" s="6"/>
+      <c r="A81" s="84" t="s">
+        <v>3198</v>
+      </c>
       <c r="B81" s="7" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
fill out github action
</commit_message>
<xml_diff>
--- a/odk/TAPE - WIP.xlsx
+++ b/odk/TAPE - WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Projects/Rstudio/tape_calculator/odk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0919CBA7-CDD7-F446-8A9D-EEE6A3620BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0612FB-A0FA-E14E-8306-AE4D165BD0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21920" yWindow="-28300" windowWidth="46080" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6224" uniqueCount="3199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6223" uniqueCount="3198">
   <si>
     <t>Comment</t>
   </si>
@@ -9700,9 +9700,6 @@
   </si>
   <si>
     <t xml:space="preserve">maybe don't need this any more? </t>
-  </si>
-  <si>
-    <t>depending on how we approach this section, this could be deleted…</t>
   </si>
 </sst>
 </file>
@@ -10835,7 +10832,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A83" sqref="A83"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -12562,9 +12559,7 @@
       <c r="O80" s="7"/>
     </row>
     <row r="81" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A81" s="84" t="s">
-        <v>3198</v>
-      </c>
+      <c r="A81" s="84"/>
       <c r="B81" s="7" t="s">
         <v>32</v>
       </c>

</xml_diff>